<commit_message>
figure and code improvements
</commit_message>
<xml_diff>
--- a/sources/cc_sectors.xlsx
+++ b/sources/cc_sectors.xlsx
@@ -9,17 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="labels" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="136">
   <si>
     <t>code</t>
   </si>
@@ -249,88 +250,184 @@
     <t>Fossil fuel fires</t>
   </si>
   <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>Waste</t>
+  </si>
+  <si>
+    <t>Buildings</t>
+  </si>
+  <si>
+    <t>1A1a</t>
+  </si>
+  <si>
+    <t>1A3</t>
+  </si>
+  <si>
+    <t>Power sector</t>
+  </si>
+  <si>
+    <t>1A2</t>
+  </si>
+  <si>
+    <t>1A4</t>
+  </si>
+  <si>
+    <t>Transport</t>
+  </si>
+  <si>
+    <t>Agriculture</t>
+  </si>
+  <si>
+    <t>Industry</t>
+  </si>
+  <si>
+    <t>3B</t>
+  </si>
+  <si>
+    <t>Land use change</t>
+  </si>
+  <si>
+    <t>3A, 3C</t>
+  </si>
+  <si>
+    <t>sector_tier_1</t>
+  </si>
+  <si>
+    <t>Energy</t>
+  </si>
+  <si>
+    <t>AFOLU</t>
+  </si>
+  <si>
+    <t>1A1bc, 1A5, 1B</t>
+  </si>
+  <si>
+    <t>sector_tier_2</t>
+  </si>
+  <si>
+    <t>sector_tier_3</t>
+  </si>
+  <si>
+    <t>sector_tier_2_codes</t>
+  </si>
+  <si>
+    <t>sector_tier_2_order</t>
+  </si>
+  <si>
+    <t>Energy|Power sector</t>
+  </si>
+  <si>
+    <t>Energy|Industry</t>
+  </si>
+  <si>
+    <t>Energy|Buildings</t>
+  </si>
+  <si>
+    <t>AFOLU|Land use change</t>
+  </si>
+  <si>
+    <t>Energy|Transport|Aviation</t>
+  </si>
+  <si>
+    <t>Energy|Transport|Road</t>
+  </si>
+  <si>
+    <t>Energy|Transport|Other</t>
+  </si>
+  <si>
+    <t>AFOLU|Agriculture|Livestock</t>
+  </si>
+  <si>
+    <t>AFOLU|Agriculture|Other</t>
+  </si>
+  <si>
+    <t>Fuel production</t>
+  </si>
+  <si>
+    <t>Energy|Fuel production &amp; other</t>
+  </si>
+  <si>
+    <t>Land use</t>
+  </si>
+  <si>
+    <t>Waste &amp; Other</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Power sector</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Industry</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Transport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Buildings</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Fuel production</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Agriculture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Land use</t>
+  </si>
+  <si>
     <t>sector</t>
   </si>
   <si>
-    <t>subsector</t>
-  </si>
-  <si>
-    <t>Other</t>
-  </si>
-  <si>
-    <t>Waste</t>
-  </si>
-  <si>
-    <t>Transport|Aviation</t>
-  </si>
-  <si>
-    <t>Transport|Road</t>
-  </si>
-  <si>
-    <t>Transport|Other</t>
-  </si>
-  <si>
-    <t>Buildings</t>
-  </si>
-  <si>
-    <t>sector_codes</t>
-  </si>
-  <si>
-    <t>1A1a</t>
-  </si>
-  <si>
-    <t>1A1bc, 1B</t>
-  </si>
-  <si>
-    <t>1A3</t>
-  </si>
-  <si>
-    <t>Power sector</t>
-  </si>
-  <si>
-    <t>1A2</t>
-  </si>
-  <si>
-    <t>1A4</t>
-  </si>
-  <si>
-    <t>Transport</t>
-  </si>
-  <si>
-    <t>Industry (process)</t>
-  </si>
-  <si>
-    <t>Agriculture</t>
-  </si>
-  <si>
-    <t>Industry (process)|Cement</t>
-  </si>
-  <si>
-    <t>Industry (process)|Other</t>
-  </si>
-  <si>
-    <t>Industry (process)|Chemicals</t>
-  </si>
-  <si>
-    <t>Industry (process)|Metals</t>
-  </si>
-  <si>
-    <t>Agriculture|Other</t>
-  </si>
-  <si>
-    <t>Agriculture|Livestock</t>
-  </si>
-  <si>
-    <t>1A5, 5</t>
-  </si>
-  <si>
-    <t>sector_order</t>
-  </si>
-  <si>
-    <t>Industry</t>
-  </si>
-  <si>
-    <t>Fossil production</t>
+    <t>position</t>
+  </si>
+  <si>
+    <t>#66c2a5</t>
+  </si>
+  <si>
+    <t>#a6d854</t>
+  </si>
+  <si>
+    <t>#fc8d62</t>
+  </si>
+  <si>
+    <t>#b3b3b3</t>
+  </si>
+  <si>
+    <t>#8da0cb</t>
+  </si>
+  <si>
+    <t>#e78ac3</t>
+  </si>
+  <si>
+    <t>#ffd92f</t>
+  </si>
+  <si>
+    <t>#e5c494</t>
+  </si>
+  <si>
+    <t>#fccde5</t>
+  </si>
+  <si>
+    <t>#ffffff</t>
+  </si>
+  <si>
+    <t>colour</t>
+  </si>
+  <si>
+    <t>Industrial processes</t>
+  </si>
+  <si>
+    <t>Industrial processes|Cement</t>
+  </si>
+  <si>
+    <t>Industrial processes|Other</t>
+  </si>
+  <si>
+    <t>Industrial processes|Chemicals</t>
+  </si>
+  <si>
+    <t>Industrial processes|Metals</t>
   </si>
 </sst>
 </file>
@@ -667,21 +764,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="77.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5703125" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" customWidth="1"/>
+    <col min="3" max="3" width="23.7109375" customWidth="1"/>
+    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -689,19 +787,22 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="D1" t="s">
-        <v>84</v>
-      </c>
-      <c r="E1" t="s">
-        <v>101</v>
+        <v>94</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>96</v>
       </c>
       <c r="F1" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+        <v>97</v>
+      </c>
+      <c r="G1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -709,19 +810,22 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="D2" t="s">
-        <v>85</v>
-      </c>
-      <c r="E2">
+        <v>81</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F2">
         <v>1</v>
       </c>
-      <c r="F2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -729,19 +833,22 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="D3" t="s">
-        <v>86</v>
-      </c>
-      <c r="E3">
-        <v>2</v>
-      </c>
-      <c r="F3" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -749,19 +856,22 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>91</v>
       </c>
       <c r="D4" t="s">
-        <v>89</v>
-      </c>
-      <c r="E4">
-        <v>5</v>
-      </c>
-      <c r="F4" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>86</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4">
+        <v>2</v>
+      </c>
+      <c r="G4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -772,16 +882,19 @@
         <v>91</v>
       </c>
       <c r="D5" t="s">
-        <v>87</v>
-      </c>
-      <c r="E5">
+        <v>84</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F5">
         <v>3</v>
       </c>
-      <c r="F5" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -792,16 +905,19 @@
         <v>91</v>
       </c>
       <c r="D6" t="s">
-        <v>87</v>
-      </c>
-      <c r="E6">
+        <v>84</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F6">
         <v>3</v>
       </c>
-      <c r="F6" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -812,16 +928,19 @@
         <v>91</v>
       </c>
       <c r="D7" t="s">
-        <v>87</v>
-      </c>
-      <c r="E7">
+        <v>84</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F7">
         <v>3</v>
       </c>
-      <c r="F7" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -832,16 +951,19 @@
         <v>91</v>
       </c>
       <c r="D8" t="s">
-        <v>87</v>
-      </c>
-      <c r="E8">
+        <v>84</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F8">
         <v>3</v>
       </c>
-      <c r="F8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -852,16 +974,19 @@
         <v>91</v>
       </c>
       <c r="D9" t="s">
-        <v>87</v>
-      </c>
-      <c r="E9">
+        <v>84</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="F9">
         <v>3</v>
       </c>
-      <c r="F9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -869,19 +994,22 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
+        <v>91</v>
+      </c>
+      <c r="D10" t="s">
+        <v>78</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="D10" t="s">
-        <v>90</v>
-      </c>
-      <c r="E10">
+      <c r="F10">
         <v>4</v>
       </c>
-      <c r="F10" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -889,19 +1017,22 @@
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>78</v>
+        <v>91</v>
       </c>
       <c r="D11" t="s">
-        <v>100</v>
-      </c>
-      <c r="E11">
-        <v>9</v>
-      </c>
-      <c r="F11" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+      <c r="G11" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -909,19 +1040,22 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="D12" t="s">
-        <v>86</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-      <c r="F12" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F12">
+        <v>5</v>
+      </c>
+      <c r="G12" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -929,19 +1063,22 @@
         <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="D13" t="s">
-        <v>86</v>
-      </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
-      <c r="F13" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="F13">
+        <v>5</v>
+      </c>
+      <c r="G13" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -949,19 +1086,22 @@
         <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>92</v>
-      </c>
-      <c r="D14" s="1">
+        <v>131</v>
+      </c>
+      <c r="D14" t="s">
+        <v>131</v>
+      </c>
+      <c r="E14" s="1">
         <v>2</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>6</v>
       </c>
-      <c r="F14" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -969,19 +1109,22 @@
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>92</v>
-      </c>
-      <c r="D15" s="1">
+        <v>131</v>
+      </c>
+      <c r="D15" t="s">
+        <v>131</v>
+      </c>
+      <c r="E15" s="1">
         <v>2</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>6</v>
       </c>
-      <c r="F15" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -989,19 +1132,22 @@
         <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>92</v>
-      </c>
-      <c r="D16" s="1">
+        <v>131</v>
+      </c>
+      <c r="D16" t="s">
+        <v>131</v>
+      </c>
+      <c r="E16" s="1">
         <v>2</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>6</v>
       </c>
-      <c r="F16" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1009,19 +1155,22 @@
         <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>92</v>
-      </c>
-      <c r="D17" s="1">
+        <v>131</v>
+      </c>
+      <c r="D17" t="s">
+        <v>131</v>
+      </c>
+      <c r="E17" s="1">
         <v>2</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>6</v>
       </c>
-      <c r="F17" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1029,19 +1178,22 @@
         <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>92</v>
-      </c>
-      <c r="D18" s="1">
+        <v>131</v>
+      </c>
+      <c r="D18" t="s">
+        <v>131</v>
+      </c>
+      <c r="E18" s="1">
         <v>2</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>6</v>
       </c>
-      <c r="F18" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G18" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1049,19 +1201,22 @@
         <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>92</v>
-      </c>
-      <c r="D19" s="1">
+        <v>131</v>
+      </c>
+      <c r="D19" t="s">
+        <v>131</v>
+      </c>
+      <c r="E19" s="1">
         <v>2</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>6</v>
       </c>
-      <c r="F19" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G19" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1069,19 +1224,22 @@
         <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>92</v>
-      </c>
-      <c r="D20" s="1">
+        <v>131</v>
+      </c>
+      <c r="D20" t="s">
+        <v>131</v>
+      </c>
+      <c r="E20" s="1">
         <v>2</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>6</v>
       </c>
-      <c r="F20" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G20" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1089,19 +1247,22 @@
         <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>92</v>
-      </c>
-      <c r="D21" s="1">
+        <v>131</v>
+      </c>
+      <c r="D21" t="s">
+        <v>131</v>
+      </c>
+      <c r="E21" s="1">
         <v>2</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>6</v>
       </c>
-      <c r="F21" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G21" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1109,19 +1270,22 @@
         <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>92</v>
-      </c>
-      <c r="D22" s="1">
+        <v>131</v>
+      </c>
+      <c r="D22" t="s">
+        <v>131</v>
+      </c>
+      <c r="E22" s="1">
         <v>2</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>6</v>
       </c>
-      <c r="F22" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G22" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -1129,19 +1293,22 @@
         <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>92</v>
-      </c>
-      <c r="D23" s="1">
+        <v>131</v>
+      </c>
+      <c r="D23" t="s">
+        <v>131</v>
+      </c>
+      <c r="E23" s="1">
         <v>2</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>6</v>
       </c>
-      <c r="F23" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1149,19 +1316,22 @@
         <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>93</v>
-      </c>
-      <c r="D24" s="1">
-        <v>3</v>
-      </c>
-      <c r="E24">
+        <v>92</v>
+      </c>
+      <c r="D24" t="s">
+        <v>85</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F24">
         <v>7</v>
       </c>
-      <c r="F24" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G24" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -1169,19 +1339,22 @@
         <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>93</v>
-      </c>
-      <c r="D25" s="1">
-        <v>3</v>
-      </c>
-      <c r="E25">
+        <v>92</v>
+      </c>
+      <c r="D25" t="s">
+        <v>85</v>
+      </c>
+      <c r="E25" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F25">
         <v>7</v>
       </c>
-      <c r="F25" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G25" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -1189,19 +1362,22 @@
         <v>51</v>
       </c>
       <c r="C26" t="s">
-        <v>93</v>
-      </c>
-      <c r="D26" s="1">
-        <v>3</v>
-      </c>
-      <c r="E26">
+        <v>92</v>
+      </c>
+      <c r="D26" t="s">
+        <v>85</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F26">
         <v>7</v>
       </c>
-      <c r="F26" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -1209,19 +1385,22 @@
         <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>93</v>
-      </c>
-      <c r="D27" s="1">
-        <v>3</v>
-      </c>
-      <c r="E27">
+        <v>92</v>
+      </c>
+      <c r="D27" t="s">
+        <v>85</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F27">
         <v>7</v>
       </c>
-      <c r="F27" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -1229,19 +1408,22 @@
         <v>55</v>
       </c>
       <c r="C28" t="s">
-        <v>93</v>
-      </c>
-      <c r="D28" s="1">
-        <v>3</v>
-      </c>
-      <c r="E28">
+        <v>92</v>
+      </c>
+      <c r="D28" t="s">
+        <v>85</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F28">
         <v>7</v>
       </c>
-      <c r="F28" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G28" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -1249,19 +1431,22 @@
         <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>93</v>
-      </c>
-      <c r="D29" s="1">
-        <v>3</v>
-      </c>
-      <c r="E29">
+        <v>92</v>
+      </c>
+      <c r="D29" t="s">
+        <v>85</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F29">
         <v>7</v>
       </c>
-      <c r="F29" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G29" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>58</v>
       </c>
@@ -1269,19 +1454,22 @@
         <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>93</v>
-      </c>
-      <c r="D30" s="1">
-        <v>3</v>
-      </c>
-      <c r="E30">
+        <v>92</v>
+      </c>
+      <c r="D30" t="s">
+        <v>85</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F30">
         <v>7</v>
       </c>
-      <c r="F30" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G30" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -1289,19 +1477,22 @@
         <v>61</v>
       </c>
       <c r="C31" t="s">
-        <v>93</v>
-      </c>
-      <c r="D31" s="1">
-        <v>3</v>
-      </c>
-      <c r="E31">
+        <v>92</v>
+      </c>
+      <c r="D31" t="s">
+        <v>85</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F31">
         <v>7</v>
       </c>
-      <c r="F31" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G31" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>62</v>
       </c>
@@ -1309,140 +1500,331 @@
         <v>63</v>
       </c>
       <c r="C32" t="s">
-        <v>93</v>
-      </c>
-      <c r="D32" s="1">
-        <v>3</v>
-      </c>
-      <c r="E32">
+        <v>92</v>
+      </c>
+      <c r="D32" t="s">
+        <v>85</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F32">
         <v>7</v>
       </c>
-      <c r="F32" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G32" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>87</v>
+      </c>
+      <c r="B33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" t="s">
+        <v>92</v>
+      </c>
+      <c r="D33" t="s">
+        <v>109</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F33">
+        <v>8</v>
+      </c>
+      <c r="G33" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
         <v>64</v>
       </c>
-      <c r="B33" t="s">
+      <c r="B34" t="s">
         <v>65</v>
       </c>
-      <c r="C33" t="s">
-        <v>79</v>
-      </c>
-      <c r="D33" s="1">
+      <c r="C34" t="s">
+        <v>110</v>
+      </c>
+      <c r="D34" t="s">
+        <v>110</v>
+      </c>
+      <c r="E34" s="1">
         <v>4</v>
       </c>
-      <c r="E33">
-        <v>8</v>
-      </c>
-      <c r="F33" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+      <c r="F34">
+        <v>9</v>
+      </c>
+      <c r="G34" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>66</v>
       </c>
-      <c r="B34" t="s">
+      <c r="B35" t="s">
         <v>67</v>
       </c>
-      <c r="C34" t="s">
-        <v>79</v>
-      </c>
-      <c r="D34" s="1">
+      <c r="C35" t="s">
+        <v>110</v>
+      </c>
+      <c r="D35" t="s">
+        <v>110</v>
+      </c>
+      <c r="E35" s="1">
         <v>4</v>
       </c>
-      <c r="E34">
-        <v>8</v>
-      </c>
-      <c r="F34" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="F35">
+        <v>9</v>
+      </c>
+      <c r="G35" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>68</v>
       </c>
-      <c r="B35" t="s">
+      <c r="B36" t="s">
         <v>69</v>
       </c>
-      <c r="C35" t="s">
-        <v>79</v>
-      </c>
-      <c r="D35" s="1">
+      <c r="C36" t="s">
+        <v>110</v>
+      </c>
+      <c r="D36" t="s">
+        <v>110</v>
+      </c>
+      <c r="E36" s="1">
         <v>4</v>
       </c>
-      <c r="E35">
-        <v>8</v>
-      </c>
-      <c r="F35" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="F36">
+        <v>9</v>
+      </c>
+      <c r="G36" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>70</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B37" t="s">
         <v>71</v>
       </c>
-      <c r="C36" t="s">
-        <v>79</v>
-      </c>
-      <c r="D36" s="1">
+      <c r="C37" t="s">
+        <v>110</v>
+      </c>
+      <c r="D37" t="s">
+        <v>110</v>
+      </c>
+      <c r="E37" s="1">
         <v>4</v>
       </c>
-      <c r="E36">
-        <v>8</v>
-      </c>
-      <c r="F36" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="F37">
+        <v>9</v>
+      </c>
+      <c r="G37" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>72</v>
       </c>
-      <c r="B37" t="s">
+      <c r="B38" t="s">
         <v>73</v>
       </c>
-      <c r="C37" t="s">
-        <v>78</v>
-      </c>
-      <c r="D37" t="s">
-        <v>100</v>
-      </c>
-      <c r="E37">
+      <c r="C38" t="s">
+        <v>110</v>
+      </c>
+      <c r="D38" t="s">
+        <v>110</v>
+      </c>
+      <c r="E38" s="1">
+        <v>5</v>
+      </c>
+      <c r="F38">
         <v>9</v>
       </c>
-      <c r="F37" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="G38" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>74</v>
       </c>
-      <c r="B38" t="s">
+      <c r="B39" t="s">
         <v>75</v>
       </c>
-      <c r="C38" t="s">
-        <v>78</v>
-      </c>
-      <c r="D38" t="s">
-        <v>100</v>
-      </c>
-      <c r="E38">
+      <c r="C39" t="s">
+        <v>110</v>
+      </c>
+      <c r="D39" t="s">
+        <v>110</v>
+      </c>
+      <c r="E39" s="1">
+        <v>5</v>
+      </c>
+      <c r="F39">
         <v>9</v>
       </c>
-      <c r="F38" t="s">
-        <v>78</v>
+      <c r="G39" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" t="s">
+        <v>119</v>
+      </c>
+      <c r="C1" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>112</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5">
+        <v>4</v>
+      </c>
+      <c r="C5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>114</v>
+      </c>
+      <c r="B6">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>115</v>
+      </c>
+      <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>131</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B9">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>116</v>
+      </c>
+      <c r="B10">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B11">
+        <v>10</v>
+      </c>
+      <c r="C11" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>110</v>
+      </c>
+      <c r="B12">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>123</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
added EU and fixed labels
</commit_message>
<xml_diff>
--- a/sources/cc_sectors.xlsx
+++ b/sources/cc_sectors.xlsx
@@ -265,9 +265,6 @@
     <t>1A3</t>
   </si>
   <si>
-    <t>Power sector</t>
-  </si>
-  <si>
     <t>1A2</t>
   </si>
   <si>
@@ -316,18 +313,12 @@
     <t>sector_tier_2_order</t>
   </si>
   <si>
-    <t>Energy|Power sector</t>
-  </si>
-  <si>
     <t>Energy|Industry</t>
   </si>
   <si>
     <t>Energy|Buildings</t>
   </si>
   <si>
-    <t>AFOLU|Land use change</t>
-  </si>
-  <si>
     <t>Energy|Transport|Aviation</t>
   </si>
   <si>
@@ -349,15 +340,9 @@
     <t>Energy|Fuel production &amp; other</t>
   </si>
   <si>
-    <t>Land use</t>
-  </si>
-  <si>
     <t>Waste &amp; Other</t>
   </si>
   <si>
-    <t xml:space="preserve">   Power sector</t>
-  </si>
-  <si>
     <t xml:space="preserve">   Industry</t>
   </si>
   <si>
@@ -373,9 +358,6 @@
     <t xml:space="preserve">   Agriculture</t>
   </si>
   <si>
-    <t xml:space="preserve">   Land use</t>
-  </si>
-  <si>
     <t>sector</t>
   </si>
   <si>
@@ -428,6 +410,24 @@
   </si>
   <si>
     <t>Industrial processes|Metals</t>
+  </si>
+  <si>
+    <t>Power</t>
+  </si>
+  <si>
+    <t>Energy|Power</t>
+  </si>
+  <si>
+    <t>LULUCF</t>
+  </si>
+  <si>
+    <t>AFOLU|LULUCF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   LULUCF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   Power</t>
   </si>
 </sst>
 </file>
@@ -767,7 +767,7 @@
   <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G20" sqref="G20"/>
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,19 +787,19 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D1" t="s">
+        <v>93</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" t="s">
+        <v>96</v>
+      </c>
+      <c r="G1" t="s">
         <v>94</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F1" t="s">
-        <v>97</v>
-      </c>
-      <c r="G1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -810,10 +810,10 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
+        <v>130</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>79</v>
@@ -822,7 +822,7 @@
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>98</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -833,19 +833,19 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F3">
         <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -856,19 +856,19 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -879,10 +879,10 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>80</v>
@@ -891,7 +891,7 @@
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -902,10 +902,10 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>80</v>
@@ -914,7 +914,7 @@
         <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -925,10 +925,10 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E7" s="1" t="s">
         <v>80</v>
@@ -937,7 +937,7 @@
         <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -948,10 +948,10 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D8" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>80</v>
@@ -960,7 +960,7 @@
         <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -971,10 +971,10 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D9" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>80</v>
@@ -983,7 +983,7 @@
         <v>3</v>
       </c>
       <c r="G9" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -994,19 +994,19 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D10" t="s">
         <v>78</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F10">
         <v>4</v>
       </c>
       <c r="G10" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1017,19 +1017,19 @@
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D11" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F11">
         <v>5</v>
       </c>
       <c r="G11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1040,19 +1040,19 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D12" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F12">
         <v>5</v>
       </c>
       <c r="G12" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1063,19 +1063,19 @@
         <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D13" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="F13">
         <v>5</v>
       </c>
       <c r="G13" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1086,10 +1086,10 @@
         <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D14" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E14" s="1">
         <v>2</v>
@@ -1098,7 +1098,7 @@
         <v>6</v>
       </c>
       <c r="G14" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1109,10 +1109,10 @@
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D15" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E15" s="1">
         <v>2</v>
@@ -1121,7 +1121,7 @@
         <v>6</v>
       </c>
       <c r="G15" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1132,10 +1132,10 @@
         <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D16" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E16" s="1">
         <v>2</v>
@@ -1144,7 +1144,7 @@
         <v>6</v>
       </c>
       <c r="G16" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
@@ -1155,10 +1155,10 @@
         <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D17" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E17" s="1">
         <v>2</v>
@@ -1167,7 +1167,7 @@
         <v>6</v>
       </c>
       <c r="G17" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1178,10 +1178,10 @@
         <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D18" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E18" s="1">
         <v>2</v>
@@ -1190,7 +1190,7 @@
         <v>6</v>
       </c>
       <c r="G18" t="s">
-        <v>134</v>
+        <v>128</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1201,10 +1201,10 @@
         <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D19" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E19" s="1">
         <v>2</v>
@@ -1213,7 +1213,7 @@
         <v>6</v>
       </c>
       <c r="G19" t="s">
-        <v>135</v>
+        <v>129</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1224,10 +1224,10 @@
         <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D20" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E20" s="1">
         <v>2</v>
@@ -1236,7 +1236,7 @@
         <v>6</v>
       </c>
       <c r="G20" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1247,10 +1247,10 @@
         <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D21" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E21" s="1">
         <v>2</v>
@@ -1259,7 +1259,7 @@
         <v>6</v>
       </c>
       <c r="G21" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1270,10 +1270,10 @@
         <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D22" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E22" s="1">
         <v>2</v>
@@ -1282,7 +1282,7 @@
         <v>6</v>
       </c>
       <c r="G22" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1293,10 +1293,10 @@
         <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D23" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="E23" s="1">
         <v>2</v>
@@ -1305,7 +1305,7 @@
         <v>6</v>
       </c>
       <c r="G23" t="s">
-        <v>133</v>
+        <v>127</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
@@ -1316,19 +1316,19 @@
         <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D24" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F24">
         <v>7</v>
       </c>
       <c r="G24" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
@@ -1339,19 +1339,19 @@
         <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D25" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F25">
         <v>7</v>
       </c>
       <c r="G25" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1362,19 +1362,19 @@
         <v>51</v>
       </c>
       <c r="C26" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D26" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F26">
         <v>7</v>
       </c>
       <c r="G26" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1385,19 +1385,19 @@
         <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D27" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F27">
         <v>7</v>
       </c>
       <c r="G27" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1408,19 +1408,19 @@
         <v>55</v>
       </c>
       <c r="C28" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D28" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F28">
         <v>7</v>
       </c>
       <c r="G28" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1431,19 +1431,19 @@
         <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D29" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E29" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F29">
         <v>7</v>
       </c>
       <c r="G29" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1454,19 +1454,19 @@
         <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D30" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F30">
         <v>7</v>
       </c>
       <c r="G30" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1477,19 +1477,19 @@
         <v>61</v>
       </c>
       <c r="C31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F31">
         <v>7</v>
       </c>
       <c r="G31" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
@@ -1500,42 +1500,42 @@
         <v>63</v>
       </c>
       <c r="C32" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D32" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F32">
         <v>7</v>
       </c>
       <c r="G32" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>86</v>
+      </c>
+      <c r="B33" t="s">
         <v>87</v>
       </c>
-      <c r="B33" t="s">
-        <v>88</v>
-      </c>
       <c r="C33" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D33" t="s">
-        <v>109</v>
+        <v>132</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="F33">
         <v>8</v>
       </c>
       <c r="G33" t="s">
-        <v>101</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1546,10 +1546,10 @@
         <v>65</v>
       </c>
       <c r="C34" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D34" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E34" s="1">
         <v>4</v>
@@ -1569,10 +1569,10 @@
         <v>67</v>
       </c>
       <c r="C35" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D35" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E35" s="1">
         <v>4</v>
@@ -1592,10 +1592,10 @@
         <v>69</v>
       </c>
       <c r="C36" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D36" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E36" s="1">
         <v>4</v>
@@ -1615,10 +1615,10 @@
         <v>71</v>
       </c>
       <c r="C37" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D37" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E37" s="1">
         <v>4</v>
@@ -1638,10 +1638,10 @@
         <v>73</v>
       </c>
       <c r="C38" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D38" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E38" s="1">
         <v>5</v>
@@ -1661,10 +1661,10 @@
         <v>75</v>
       </c>
       <c r="C39" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D39" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E39" s="1">
         <v>5</v>
@@ -1687,141 +1687,141 @@
   <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="B1" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="C1" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>111</v>
+        <v>135</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>117</v>
+        <v>134</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed formats, added zip
</commit_message>
<xml_diff>
--- a/sources/cc_sectors.xlsx
+++ b/sources/cc_sectors.xlsx
@@ -9,18 +9,18 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="13125" windowHeight="6105" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13130" windowHeight="6110" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
-    <sheet name="labels" sheetId="2" r:id="rId2"/>
+    <sheet name="sectors" sheetId="1" r:id="rId1"/>
+    <sheet name="labels" sheetId="3" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="137">
   <si>
     <t>code</t>
   </si>
@@ -256,9 +256,6 @@
     <t>Waste</t>
   </si>
   <si>
-    <t>Buildings</t>
-  </si>
-  <si>
     <t>1A1a</t>
   </si>
   <si>
@@ -271,15 +268,6 @@
     <t>1A4</t>
   </si>
   <si>
-    <t>Transport</t>
-  </si>
-  <si>
-    <t>Agriculture</t>
-  </si>
-  <si>
-    <t>Industry</t>
-  </si>
-  <si>
     <t>3B</t>
   </si>
   <si>
@@ -289,9 +277,6 @@
     <t>3A, 3C</t>
   </si>
   <si>
-    <t>sector_tier_1</t>
-  </si>
-  <si>
     <t>Energy</t>
   </si>
   <si>
@@ -301,18 +286,9 @@
     <t>1A1bc, 1A5, 1B</t>
   </si>
   <si>
-    <t>sector_tier_2</t>
-  </si>
-  <si>
     <t>sector_tier_3</t>
   </si>
   <si>
-    <t>sector_tier_2_codes</t>
-  </si>
-  <si>
-    <t>sector_tier_2_order</t>
-  </si>
-  <si>
     <t>Energy|Industry</t>
   </si>
   <si>
@@ -334,30 +310,12 @@
     <t>AFOLU|Agriculture|Other</t>
   </si>
   <si>
-    <t>Fuel production</t>
-  </si>
-  <si>
     <t>Energy|Fuel production &amp; other</t>
   </si>
   <si>
     <t>Waste &amp; Other</t>
   </si>
   <si>
-    <t xml:space="preserve">   Industry</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Transport</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Buildings</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Fuel production</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Agriculture</t>
-  </si>
-  <si>
     <t>sector</t>
   </si>
   <si>
@@ -391,9 +349,6 @@
     <t>#fccde5</t>
   </si>
   <si>
-    <t>#ffffff</t>
-  </si>
-  <si>
     <t>colour</t>
   </si>
   <si>
@@ -412,22 +367,70 @@
     <t>Industrial processes|Metals</t>
   </si>
   <si>
-    <t>Power</t>
-  </si>
-  <si>
     <t>Energy|Power</t>
   </si>
   <si>
-    <t>LULUCF</t>
-  </si>
-  <si>
     <t>AFOLU|LULUCF</t>
   </si>
   <si>
-    <t xml:space="preserve">   LULUCF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   Power</t>
+    <t>icons</t>
+  </si>
+  <si>
+    <t>C:/Users/lamw/ownCloud/Projects/UNEP Gap Report 2024/sources/icons/Power.png</t>
+  </si>
+  <si>
+    <t>C:/Users/lamw/ownCloud/Projects/UNEP Gap Report 2024/sources/icons/Industry.png</t>
+  </si>
+  <si>
+    <t>C:/Users/lamw/ownCloud/Projects/UNEP Gap Report 2024/sources/icons/Transport.png</t>
+  </si>
+  <si>
+    <t>C:/Users/lamw/ownCloud/Projects/UNEP Gap Report 2024/sources/icons/Buildings.png</t>
+  </si>
+  <si>
+    <t>C:/Users/lamw/ownCloud/Projects/UNEP Gap Report 2024/sources/icons/Fuel production.png</t>
+  </si>
+  <si>
+    <t>C:/Users/lamw/ownCloud/Projects/UNEP Gap Report 2024/sources/icons/Industrial processes.png</t>
+  </si>
+  <si>
+    <t>C:/Users/lamw/ownCloud/Projects/UNEP Gap Report 2024/sources/icons/Agriculture.png</t>
+  </si>
+  <si>
+    <t>C:/Users/lamw/ownCloud/Projects/UNEP Gap Report 2024/sources/icons/Waste &amp; Other.png</t>
+  </si>
+  <si>
+    <t>Energy: Power</t>
+  </si>
+  <si>
+    <t>Energy: Fuel production</t>
+  </si>
+  <si>
+    <t>Energy: Industry</t>
+  </si>
+  <si>
+    <t>Energy: Transport</t>
+  </si>
+  <si>
+    <t>Energy: Buildings</t>
+  </si>
+  <si>
+    <t>AFOLU: Agriculture</t>
+  </si>
+  <si>
+    <t>AFOLU: Land use</t>
+  </si>
+  <si>
+    <t>subsector</t>
+  </si>
+  <si>
+    <t>subsector_codes</t>
+  </si>
+  <si>
+    <t>subsector_order</t>
+  </si>
+  <si>
+    <t>C:/Users/lamw/ownCloud/Projects/UNEP Gap Report 2024/sources/icons/Land use.png</t>
   </si>
 </sst>
 </file>
@@ -766,20 +769,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G34" sqref="G34"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="77.28515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.7109375" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="77.26953125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="23.7265625" customWidth="1"/>
+    <col min="4" max="4" width="26.81640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -787,22 +790,22 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
       <c r="D1" t="s">
-        <v>93</v>
+        <v>133</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>95</v>
+        <v>134</v>
       </c>
       <c r="F1" t="s">
-        <v>96</v>
+        <v>135</v>
       </c>
       <c r="G1" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -810,22 +813,22 @@
         <v>3</v>
       </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D2" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
       <c r="G2" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -833,22 +836,22 @@
         <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D3" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F3">
         <v>5</v>
       </c>
       <c r="G3" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -856,22 +859,22 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D4" t="s">
-        <v>85</v>
+        <v>128</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F4">
         <v>2</v>
       </c>
       <c r="G4" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -879,22 +882,22 @@
         <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D5" t="s">
-        <v>83</v>
+        <v>129</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F5">
         <v>3</v>
       </c>
       <c r="G5" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
@@ -902,22 +905,22 @@
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D6" t="s">
-        <v>83</v>
+        <v>129</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F6">
         <v>3</v>
       </c>
       <c r="G6" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
@@ -925,22 +928,22 @@
         <v>13</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D7" t="s">
-        <v>83</v>
+        <v>129</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F7">
         <v>3</v>
       </c>
       <c r="G7" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -948,22 +951,22 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D8" t="s">
-        <v>83</v>
+        <v>129</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F8">
         <v>3</v>
       </c>
       <c r="G8" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -971,22 +974,22 @@
         <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D9" t="s">
-        <v>83</v>
+        <v>129</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F9">
         <v>3</v>
       </c>
       <c r="G9" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>18</v>
       </c>
@@ -994,22 +997,22 @@
         <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D10" t="s">
-        <v>78</v>
+        <v>130</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F10">
         <v>4</v>
       </c>
       <c r="G10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -1017,22 +1020,22 @@
         <v>21</v>
       </c>
       <c r="C11" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D11" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F11">
         <v>5</v>
       </c>
       <c r="G11" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>22</v>
       </c>
@@ -1040,22 +1043,22 @@
         <v>23</v>
       </c>
       <c r="C12" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D12" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F12">
         <v>5</v>
       </c>
       <c r="G12" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>24</v>
       </c>
@@ -1063,22 +1066,22 @@
         <v>25</v>
       </c>
       <c r="C13" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D13" t="s">
-        <v>104</v>
+        <v>127</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="F13">
         <v>5</v>
       </c>
       <c r="G13" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1086,10 +1089,10 @@
         <v>27</v>
       </c>
       <c r="C14" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="D14" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="E14" s="1">
         <v>2</v>
@@ -1098,10 +1101,10 @@
         <v>6</v>
       </c>
       <c r="G14" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>28</v>
       </c>
@@ -1109,10 +1112,10 @@
         <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="D15" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="E15" s="1">
         <v>2</v>
@@ -1121,10 +1124,10 @@
         <v>6</v>
       </c>
       <c r="G15" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>30</v>
       </c>
@@ -1132,10 +1135,10 @@
         <v>31</v>
       </c>
       <c r="C16" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="D16" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="E16" s="1">
         <v>2</v>
@@ -1144,10 +1147,10 @@
         <v>6</v>
       </c>
       <c r="G16" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>32</v>
       </c>
@@ -1155,10 +1158,10 @@
         <v>33</v>
       </c>
       <c r="C17" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="D17" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="E17" s="1">
         <v>2</v>
@@ -1167,10 +1170,10 @@
         <v>6</v>
       </c>
       <c r="G17" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>34</v>
       </c>
@@ -1178,10 +1181,10 @@
         <v>35</v>
       </c>
       <c r="C18" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="D18" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="E18" s="1">
         <v>2</v>
@@ -1190,10 +1193,10 @@
         <v>6</v>
       </c>
       <c r="G18" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>36</v>
       </c>
@@ -1201,10 +1204,10 @@
         <v>37</v>
       </c>
       <c r="C19" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="D19" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="E19" s="1">
         <v>2</v>
@@ -1213,10 +1216,10 @@
         <v>6</v>
       </c>
       <c r="G19" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>38</v>
       </c>
@@ -1224,10 +1227,10 @@
         <v>39</v>
       </c>
       <c r="C20" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="D20" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="E20" s="1">
         <v>2</v>
@@ -1236,10 +1239,10 @@
         <v>6</v>
       </c>
       <c r="G20" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>40</v>
       </c>
@@ -1247,10 +1250,10 @@
         <v>41</v>
       </c>
       <c r="C21" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="D21" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="E21" s="1">
         <v>2</v>
@@ -1259,10 +1262,10 @@
         <v>6</v>
       </c>
       <c r="G21" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>42</v>
       </c>
@@ -1270,10 +1273,10 @@
         <v>43</v>
       </c>
       <c r="C22" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="D22" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="E22" s="1">
         <v>2</v>
@@ -1282,10 +1285,10 @@
         <v>6</v>
       </c>
       <c r="G22" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
         <v>44</v>
       </c>
@@ -1293,10 +1296,10 @@
         <v>45</v>
       </c>
       <c r="C23" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="D23" t="s">
-        <v>125</v>
+        <v>110</v>
       </c>
       <c r="E23" s="1">
         <v>2</v>
@@ -1305,10 +1308,10 @@
         <v>6</v>
       </c>
       <c r="G23" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>46</v>
       </c>
@@ -1316,22 +1319,22 @@
         <v>47</v>
       </c>
       <c r="C24" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D24" t="s">
+        <v>131</v>
+      </c>
+      <c r="E24" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="F24">
         <v>7</v>
       </c>
       <c r="G24" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
         <v>48</v>
       </c>
@@ -1339,22 +1342,22 @@
         <v>49</v>
       </c>
       <c r="C25" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D25" t="s">
+        <v>131</v>
+      </c>
+      <c r="E25" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="E25" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="F25">
         <v>7</v>
       </c>
       <c r="G25" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
         <v>50</v>
       </c>
@@ -1362,22 +1365,22 @@
         <v>51</v>
       </c>
       <c r="C26" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D26" t="s">
+        <v>131</v>
+      </c>
+      <c r="E26" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="E26" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="F26">
         <v>7</v>
       </c>
       <c r="G26" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
         <v>52</v>
       </c>
@@ -1385,22 +1388,22 @@
         <v>53</v>
       </c>
       <c r="C27" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D27" t="s">
+        <v>131</v>
+      </c>
+      <c r="E27" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="E27" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="F27">
         <v>7</v>
       </c>
       <c r="G27" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
         <v>54</v>
       </c>
@@ -1408,22 +1411,22 @@
         <v>55</v>
       </c>
       <c r="C28" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D28" t="s">
+        <v>131</v>
+      </c>
+      <c r="E28" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="E28" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="F28">
         <v>7</v>
       </c>
       <c r="G28" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
         <v>56</v>
       </c>
@@ -1431,22 +1434,22 @@
         <v>57</v>
       </c>
       <c r="C29" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D29" t="s">
+        <v>131</v>
+      </c>
+      <c r="E29" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="F29">
         <v>7</v>
       </c>
       <c r="G29" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
         <v>58</v>
       </c>
@@ -1454,22 +1457,22 @@
         <v>59</v>
       </c>
       <c r="C30" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D30" t="s">
+        <v>131</v>
+      </c>
+      <c r="E30" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="F30">
         <v>7</v>
       </c>
       <c r="G30" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
         <v>60</v>
       </c>
@@ -1477,22 +1480,22 @@
         <v>61</v>
       </c>
       <c r="C31" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D31" t="s">
+        <v>131</v>
+      </c>
+      <c r="E31" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="F31">
         <v>7</v>
       </c>
       <c r="G31" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
         <v>62</v>
       </c>
@@ -1500,45 +1503,45 @@
         <v>63</v>
       </c>
       <c r="C32" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D32" t="s">
+        <v>131</v>
+      </c>
+      <c r="E32" s="1" t="s">
         <v>84</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="F32">
         <v>7</v>
       </c>
       <c r="G32" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
+        <v>82</v>
+      </c>
+      <c r="B33" t="s">
+        <v>83</v>
+      </c>
+      <c r="C33" t="s">
         <v>86</v>
-      </c>
-      <c r="B33" t="s">
-        <v>87</v>
-      </c>
-      <c r="C33" t="s">
-        <v>91</v>
       </c>
       <c r="D33" t="s">
         <v>132</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F33">
         <v>8</v>
       </c>
       <c r="G33" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
         <v>64</v>
       </c>
@@ -1546,10 +1549,10 @@
         <v>65</v>
       </c>
       <c r="C34" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D34" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E34" s="1">
         <v>4</v>
@@ -1561,7 +1564,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
         <v>66</v>
       </c>
@@ -1569,10 +1572,10 @@
         <v>67</v>
       </c>
       <c r="C35" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D35" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E35" s="1">
         <v>4</v>
@@ -1584,7 +1587,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
         <v>68</v>
       </c>
@@ -1592,10 +1595,10 @@
         <v>69</v>
       </c>
       <c r="C36" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D36" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E36" s="1">
         <v>4</v>
@@ -1607,7 +1610,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
         <v>70</v>
       </c>
@@ -1615,10 +1618,10 @@
         <v>71</v>
       </c>
       <c r="C37" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D37" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E37" s="1">
         <v>4</v>
@@ -1630,7 +1633,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
         <v>72</v>
       </c>
@@ -1638,10 +1641,10 @@
         <v>73</v>
       </c>
       <c r="C38" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D38" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E38" s="1">
         <v>5</v>
@@ -1653,7 +1656,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
         <v>74</v>
       </c>
@@ -1661,10 +1664,10 @@
         <v>75</v>
       </c>
       <c r="C39" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="D39" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="E39" s="1">
         <v>5</v>
@@ -1684,81 +1687,102 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18.1796875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>112</v>
+        <v>133</v>
       </c>
       <c r="B1" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+      <c r="D1" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>126</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+      <c r="D2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>104</v>
+      </c>
+      <c r="D3" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>129</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+        <v>105</v>
+      </c>
+      <c r="D4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>130</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+        <v>106</v>
+      </c>
+      <c r="D5" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>127</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+        <v>107</v>
+      </c>
+      <c r="D6" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>110</v>
       </c>
@@ -1766,62 +1790,52 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+      <c r="D7" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>125</v>
+        <v>131</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+      <c r="D8" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>91</v>
+        <v>132</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+      <c r="D9" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>106</v>
-      </c>
-      <c r="B12">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>117</v>
+        <v>103</v>
+      </c>
+      <c r="D10" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update LDCs, fix EDGAR link
</commit_message>
<xml_diff>
--- a/sources/cc_sectors.xlsx
+++ b/sources/cc_sectors.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamw\ownCloud\Projects\UNEP Gap Report 2024\sources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lamw\ownCloud\Projects\UNEP-Gap-Report-2024-Chapter-2\sources\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -312,30 +312,6 @@
     <t>Industrial processes</t>
   </si>
   <si>
-    <t>C:/Users/lamw/ownCloud/Projects/UNEP Gap Report 2024/sources/icons/Power.png</t>
-  </si>
-  <si>
-    <t>C:/Users/lamw/ownCloud/Projects/UNEP Gap Report 2024/sources/icons/Industry.png</t>
-  </si>
-  <si>
-    <t>C:/Users/lamw/ownCloud/Projects/UNEP Gap Report 2024/sources/icons/Transport.png</t>
-  </si>
-  <si>
-    <t>C:/Users/lamw/ownCloud/Projects/UNEP Gap Report 2024/sources/icons/Buildings.png</t>
-  </si>
-  <si>
-    <t>C:/Users/lamw/ownCloud/Projects/UNEP Gap Report 2024/sources/icons/Fuel production.png</t>
-  </si>
-  <si>
-    <t>C:/Users/lamw/ownCloud/Projects/UNEP Gap Report 2024/sources/icons/Industrial processes.png</t>
-  </si>
-  <si>
-    <t>C:/Users/lamw/ownCloud/Projects/UNEP Gap Report 2024/sources/icons/Agriculture.png</t>
-  </si>
-  <si>
-    <t>C:/Users/lamw/ownCloud/Projects/UNEP Gap Report 2024/sources/icons/Waste &amp; Other.png</t>
-  </si>
-  <si>
     <t>Energy: Power</t>
   </si>
   <si>
@@ -354,9 +330,6 @@
     <t>AFOLU: Agriculture</t>
   </si>
   <si>
-    <t>C:/Users/lamw/ownCloud/Projects/UNEP Gap Report 2024/sources/icons/Land use.png</t>
-  </si>
-  <si>
     <t>Power</t>
   </si>
   <si>
@@ -508,6 +481,33 @@
   </si>
   <si>
     <t>Cement (excl. carbonation)</t>
+  </si>
+  <si>
+    <t>C:/Users/lamw/ownCloud/Projects/UNEP-Gap-Report-2024-Chapter-2/sources/icons/Power.png</t>
+  </si>
+  <si>
+    <t>C:/Users/lamw/ownCloud/Projects/UNEP-Gap-Report-2024-Chapter-2/sources/icons/Fuel production.png</t>
+  </si>
+  <si>
+    <t>C:/Users/lamw/ownCloud/Projects/UNEP-Gap-Report-2024-Chapter-2/sources/icons/Industry.png</t>
+  </si>
+  <si>
+    <t>C:/Users/lamw/ownCloud/Projects/UNEP-Gap-Report-2024-Chapter-2/sources/icons/Transport.png</t>
+  </si>
+  <si>
+    <t>C:/Users/lamw/ownCloud/Projects/UNEP-Gap-Report-2024-Chapter-2/sources/icons/Buildings.png</t>
+  </si>
+  <si>
+    <t>C:/Users/lamw/ownCloud/Projects/UNEP-Gap-Report-2024-Chapter-2/sources/icons/Industrial processes.png</t>
+  </si>
+  <si>
+    <t>C:/Users/lamw/ownCloud/Projects/UNEP-Gap-Report-2024-Chapter-2/sources/icons/Agriculture.png</t>
+  </si>
+  <si>
+    <t>C:/Users/lamw/ownCloud/Projects/UNEP-Gap-Report-2024-Chapter-2/sources/icons/Land use.png</t>
+  </si>
+  <si>
+    <t>C:/Users/lamw/ownCloud/Projects/UNEP-Gap-Report-2024-Chapter-2/sources/icons/Waste &amp; Other.png</t>
   </si>
 </sst>
 </file>
@@ -847,7 +847,7 @@
   <dimension ref="A1:L41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,7 +855,9 @@
     <col min="2" max="2" width="51.140625" customWidth="1"/>
     <col min="3" max="3" width="23.7109375" customWidth="1"/>
     <col min="4" max="4" width="14.42578125" customWidth="1"/>
-    <col min="5" max="9" width="16.85546875" customWidth="1"/>
+    <col min="5" max="7" width="16.85546875" customWidth="1"/>
+    <col min="8" max="8" width="48.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16.85546875" customWidth="1"/>
     <col min="10" max="10" width="28.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -867,34 +869,34 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D1" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="E1" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="F1" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="G1" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="H1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="I1" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="J1" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="K1" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="L1" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -911,7 +913,7 @@
         <v>1</v>
       </c>
       <c r="E2" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="F2">
         <v>1</v>
@@ -920,13 +922,13 @@
         <v>89</v>
       </c>
       <c r="H2" t="s">
-        <v>97</v>
+        <v>154</v>
       </c>
       <c r="I2" t="s">
         <v>76</v>
       </c>
       <c r="J2" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>76</v>
@@ -949,7 +951,7 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F3">
         <v>5</v>
@@ -958,16 +960,16 @@
         <v>94</v>
       </c>
       <c r="H3" t="s">
-        <v>101</v>
+        <v>155</v>
       </c>
       <c r="I3" t="s">
         <v>85</v>
       </c>
       <c r="J3" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="L3">
         <v>8</v>
@@ -987,7 +989,7 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="F4">
         <v>2</v>
@@ -996,13 +998,13 @@
         <v>91</v>
       </c>
       <c r="H4" t="s">
-        <v>98</v>
+        <v>156</v>
       </c>
       <c r="I4" t="s">
         <v>78</v>
       </c>
       <c r="J4" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="K4" s="1" t="s">
         <v>78</v>
@@ -1025,7 +1027,7 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -1034,16 +1036,16 @@
         <v>92</v>
       </c>
       <c r="H5" t="s">
-        <v>99</v>
+        <v>157</v>
       </c>
       <c r="I5" t="s">
         <v>77</v>
       </c>
       <c r="J5" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="K5" s="1" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="L5">
         <v>3</v>
@@ -1063,7 +1065,7 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="F6">
         <v>3</v>
@@ -1072,16 +1074,16 @@
         <v>92</v>
       </c>
       <c r="H6" t="s">
-        <v>99</v>
+        <v>157</v>
       </c>
       <c r="I6" t="s">
         <v>77</v>
       </c>
       <c r="J6" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="L6">
         <v>4</v>
@@ -1101,7 +1103,7 @@
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="F7">
         <v>3</v>
@@ -1110,16 +1112,16 @@
         <v>92</v>
       </c>
       <c r="H7" t="s">
-        <v>99</v>
+        <v>157</v>
       </c>
       <c r="I7" t="s">
         <v>77</v>
       </c>
       <c r="J7" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="L7">
         <v>5</v>
@@ -1139,7 +1141,7 @@
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="F8">
         <v>3</v>
@@ -1148,16 +1150,16 @@
         <v>92</v>
       </c>
       <c r="H8" t="s">
-        <v>99</v>
+        <v>157</v>
       </c>
       <c r="I8" t="s">
         <v>77</v>
       </c>
       <c r="J8" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="L8">
         <v>5</v>
@@ -1177,7 +1179,7 @@
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="F9">
         <v>3</v>
@@ -1186,16 +1188,16 @@
         <v>92</v>
       </c>
       <c r="H9" t="s">
-        <v>99</v>
+        <v>157</v>
       </c>
       <c r="I9" t="s">
         <v>77</v>
       </c>
       <c r="J9" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="L9">
         <v>5</v>
@@ -1215,7 +1217,7 @@
         <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="F10">
         <v>4</v>
@@ -1224,13 +1226,13 @@
         <v>93</v>
       </c>
       <c r="H10" t="s">
-        <v>100</v>
+        <v>158</v>
       </c>
       <c r="I10" t="s">
         <v>79</v>
       </c>
       <c r="J10" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="K10" s="1" t="s">
         <v>79</v>
@@ -1253,7 +1255,7 @@
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F11">
         <v>5</v>
@@ -1262,16 +1264,16 @@
         <v>94</v>
       </c>
       <c r="H11" t="s">
-        <v>101</v>
+        <v>155</v>
       </c>
       <c r="I11" t="s">
         <v>85</v>
       </c>
       <c r="J11" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="L11">
         <v>8</v>
@@ -1291,7 +1293,7 @@
         <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F12">
         <v>5</v>
@@ -1300,16 +1302,16 @@
         <v>94</v>
       </c>
       <c r="H12" t="s">
-        <v>101</v>
+        <v>155</v>
       </c>
       <c r="I12" t="s">
         <v>85</v>
       </c>
       <c r="J12" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="K12" s="1" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="L12">
         <v>7</v>
@@ -1329,7 +1331,7 @@
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="F13">
         <v>5</v>
@@ -1338,16 +1340,16 @@
         <v>94</v>
       </c>
       <c r="H13" t="s">
-        <v>101</v>
+        <v>155</v>
       </c>
       <c r="I13" t="s">
         <v>85</v>
       </c>
       <c r="J13" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="K13" s="1" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="L13">
         <v>7</v>
@@ -1376,16 +1378,16 @@
         <v>95</v>
       </c>
       <c r="H14" t="s">
-        <v>102</v>
+        <v>159</v>
       </c>
       <c r="I14" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="J14" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="K14" s="1" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="L14">
         <v>9</v>
@@ -1393,10 +1395,10 @@
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="B15" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C15" t="s">
         <v>96</v>
@@ -1414,16 +1416,16 @@
         <v>95</v>
       </c>
       <c r="H15" t="s">
-        <v>102</v>
+        <v>159</v>
       </c>
       <c r="I15" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="J15" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="K15" s="1" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="L15">
         <v>9</v>
@@ -1452,16 +1454,16 @@
         <v>95</v>
       </c>
       <c r="H16" t="s">
-        <v>102</v>
+        <v>159</v>
       </c>
       <c r="I16" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="J16" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="K16" s="1" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="L16">
         <v>12</v>
@@ -1490,16 +1492,16 @@
         <v>95</v>
       </c>
       <c r="H17" t="s">
-        <v>102</v>
+        <v>159</v>
       </c>
       <c r="I17" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="J17" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="K17" s="1" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="L17">
         <v>12</v>
@@ -1528,16 +1530,16 @@
         <v>95</v>
       </c>
       <c r="H18" t="s">
-        <v>102</v>
+        <v>159</v>
       </c>
       <c r="I18" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="J18" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="K18" s="1" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="L18">
         <v>12</v>
@@ -1566,16 +1568,16 @@
         <v>95</v>
       </c>
       <c r="H19" t="s">
-        <v>102</v>
+        <v>159</v>
       </c>
       <c r="I19" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="J19" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="K19" s="1" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="L19">
         <v>10</v>
@@ -1604,16 +1606,16 @@
         <v>95</v>
       </c>
       <c r="H20" t="s">
-        <v>102</v>
+        <v>159</v>
       </c>
       <c r="I20" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="J20" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="K20" s="1" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="L20">
         <v>11</v>
@@ -1642,16 +1644,16 @@
         <v>95</v>
       </c>
       <c r="H21" t="s">
-        <v>102</v>
+        <v>159</v>
       </c>
       <c r="I21" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="J21" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="K21" s="1" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="L21">
         <v>12</v>
@@ -1680,16 +1682,16 @@
         <v>95</v>
       </c>
       <c r="H22" t="s">
-        <v>102</v>
+        <v>159</v>
       </c>
       <c r="I22" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="J22" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="K22" s="1" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="L22">
         <v>12</v>
@@ -1718,16 +1720,16 @@
         <v>95</v>
       </c>
       <c r="H23" t="s">
-        <v>102</v>
+        <v>159</v>
       </c>
       <c r="I23" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="J23" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="K23" s="1" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="L23">
         <v>12</v>
@@ -1756,16 +1758,16 @@
         <v>95</v>
       </c>
       <c r="H24" t="s">
-        <v>102</v>
+        <v>159</v>
       </c>
       <c r="I24" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="J24" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="K24" s="1" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="L24">
         <v>12</v>
@@ -1785,7 +1787,7 @@
         <v>3</v>
       </c>
       <c r="E25" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="F25">
         <v>7</v>
@@ -1794,16 +1796,16 @@
         <v>87</v>
       </c>
       <c r="H25" t="s">
-        <v>103</v>
+        <v>160</v>
       </c>
       <c r="I25" t="s">
         <v>82</v>
       </c>
       <c r="J25" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="K25" s="1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="L25">
         <v>13</v>
@@ -1823,7 +1825,7 @@
         <v>3</v>
       </c>
       <c r="E26" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="F26">
         <v>7</v>
@@ -1832,16 +1834,16 @@
         <v>87</v>
       </c>
       <c r="H26" t="s">
-        <v>103</v>
+        <v>160</v>
       </c>
       <c r="I26" t="s">
         <v>82</v>
       </c>
       <c r="J26" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="K26" s="1" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="L26">
         <v>13</v>
@@ -1861,7 +1863,7 @@
         <v>3</v>
       </c>
       <c r="E27" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="F27">
         <v>7</v>
@@ -1870,16 +1872,16 @@
         <v>87</v>
       </c>
       <c r="H27" t="s">
-        <v>103</v>
+        <v>160</v>
       </c>
       <c r="I27" t="s">
         <v>82</v>
       </c>
       <c r="J27" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="K27" s="1" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="L27">
         <v>14</v>
@@ -1899,7 +1901,7 @@
         <v>3</v>
       </c>
       <c r="E28" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="F28">
         <v>7</v>
@@ -1908,16 +1910,16 @@
         <v>87</v>
       </c>
       <c r="H28" t="s">
-        <v>103</v>
+        <v>160</v>
       </c>
       <c r="I28" t="s">
         <v>82</v>
       </c>
       <c r="J28" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="K28" s="1" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="L28">
         <v>14</v>
@@ -1937,7 +1939,7 @@
         <v>3</v>
       </c>
       <c r="E29" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="F29">
         <v>7</v>
@@ -1946,16 +1948,16 @@
         <v>87</v>
       </c>
       <c r="H29" t="s">
-        <v>103</v>
+        <v>160</v>
       </c>
       <c r="I29" t="s">
         <v>82</v>
       </c>
       <c r="J29" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="K29" s="1" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="L29">
         <v>14</v>
@@ -1975,7 +1977,7 @@
         <v>3</v>
       </c>
       <c r="E30" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="F30">
         <v>7</v>
@@ -1984,16 +1986,16 @@
         <v>87</v>
       </c>
       <c r="H30" t="s">
-        <v>103</v>
+        <v>160</v>
       </c>
       <c r="I30" t="s">
         <v>82</v>
       </c>
       <c r="J30" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="K30" s="1" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="L30">
         <v>14</v>
@@ -2013,7 +2015,7 @@
         <v>3</v>
       </c>
       <c r="E31" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="F31">
         <v>7</v>
@@ -2022,16 +2024,16 @@
         <v>87</v>
       </c>
       <c r="H31" t="s">
-        <v>103</v>
+        <v>160</v>
       </c>
       <c r="I31" t="s">
         <v>82</v>
       </c>
       <c r="J31" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="L31">
         <v>14</v>
@@ -2051,7 +2053,7 @@
         <v>3</v>
       </c>
       <c r="E32" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="F32">
         <v>7</v>
@@ -2060,16 +2062,16 @@
         <v>87</v>
       </c>
       <c r="H32" t="s">
-        <v>103</v>
+        <v>160</v>
       </c>
       <c r="I32" t="s">
         <v>82</v>
       </c>
       <c r="J32" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="K32" s="1" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="L32">
         <v>14</v>
@@ -2089,7 +2091,7 @@
         <v>3</v>
       </c>
       <c r="E33" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="F33">
         <v>7</v>
@@ -2098,16 +2100,16 @@
         <v>87</v>
       </c>
       <c r="H33" t="s">
-        <v>103</v>
+        <v>160</v>
       </c>
       <c r="I33" t="s">
         <v>82</v>
       </c>
       <c r="J33" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="K33" s="1" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="L33">
         <v>14</v>
@@ -2127,7 +2129,7 @@
         <v>3</v>
       </c>
       <c r="E34" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F34">
         <v>8</v>
@@ -2136,13 +2138,13 @@
         <v>88</v>
       </c>
       <c r="H34" t="s">
+        <v>161</v>
+      </c>
+      <c r="I34" t="s">
+        <v>148</v>
+      </c>
+      <c r="J34" t="s">
         <v>111</v>
-      </c>
-      <c r="I34" t="s">
-        <v>157</v>
-      </c>
-      <c r="J34" t="s">
-        <v>120</v>
       </c>
       <c r="K34" s="1" t="s">
         <v>80</v>
@@ -2153,10 +2155,10 @@
     </row>
     <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B35" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C35" t="s">
         <v>84</v>
@@ -2165,7 +2167,7 @@
         <v>3</v>
       </c>
       <c r="E35" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="F35">
         <v>8</v>
@@ -2174,16 +2176,16 @@
         <v>88</v>
       </c>
       <c r="H35" t="s">
-        <v>111</v>
+        <v>161</v>
       </c>
       <c r="I35" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="J35" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="K35" s="1" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="L35">
         <v>16</v>
@@ -2212,16 +2214,16 @@
         <v>90</v>
       </c>
       <c r="H36" t="s">
-        <v>104</v>
+        <v>162</v>
       </c>
       <c r="I36" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="J36" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="K36" s="1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="L36">
         <v>17</v>
@@ -2250,16 +2252,16 @@
         <v>90</v>
       </c>
       <c r="H37" t="s">
-        <v>104</v>
+        <v>162</v>
       </c>
       <c r="I37" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="J37" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="K37" s="1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="L37">
         <v>17</v>
@@ -2288,16 +2290,16 @@
         <v>90</v>
       </c>
       <c r="H38" t="s">
-        <v>104</v>
+        <v>162</v>
       </c>
       <c r="I38" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="J38" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="K38" s="1" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="L38">
         <v>17</v>
@@ -2326,16 +2328,16 @@
         <v>90</v>
       </c>
       <c r="H39" t="s">
-        <v>104</v>
+        <v>162</v>
       </c>
       <c r="I39" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="J39" t="s">
+        <v>113</v>
+      </c>
+      <c r="K39" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="K39" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="L39">
         <v>18</v>
@@ -2364,13 +2366,13 @@
         <v>90</v>
       </c>
       <c r="H40" t="s">
-        <v>104</v>
+        <v>162</v>
       </c>
       <c r="I40" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="J40" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="K40" s="1">
         <v>5</v>
@@ -2402,13 +2404,13 @@
         <v>90</v>
       </c>
       <c r="H41" t="s">
-        <v>104</v>
+        <v>162</v>
       </c>
       <c r="I41" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="J41" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="K41" s="1">
         <v>5</v>

</xml_diff>